<commit_message>
Add tracked packages to Secured Mail Manifest file.
</commit_message>
<xml_diff>
--- a/spring_manifest/views/file_manifest/secure_mail_manifest_template.xlsx
+++ b/spring_manifest/views/file_manifest/secure_mail_manifest_template.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Instructions" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Priority Mail'!$A$1:$X$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Priority Mail'!$A$1:$X$23</definedName>
     <definedName function="false" hidden="false" name="CountryList" vbProcedure="false">data!#ref!</definedName>
     <definedName function="false" hidden="false" name="Format" vbProcedure="false">data!#ref!</definedName>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t xml:space="preserve">International Manifest</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rest of World</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracked</t>
   </si>
   <si>
     <t xml:space="preserve">Sub Totals</t>
@@ -193,7 +196,7 @@
     <numFmt numFmtId="173" formatCode="\£#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.00"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -217,8 +220,124 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF339966"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFED722A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FF666699"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF339966"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FF339966"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF259AC4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FFED722A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00759B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF00759B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FFED722A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FFED722A"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -226,128 +345,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF339966"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFED722A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FF666699"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF339966"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FF339966"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF259AC4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FFED722A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF00759B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF00759B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFED722A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FFED722A"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -538,7 +535,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,23 +561,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -589,11 +578,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -601,8 +590,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -618,242 +615,226 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="31" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="32" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="32" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="32" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="33" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="33" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="33" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="33" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="33" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="4" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="29" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="174" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="34" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -861,7 +842,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -869,11 +850,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -886,16 +867,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_Zoning 0.1" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="5">
@@ -999,7 +978,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1494000</xdr:colOff>
+      <xdr:colOff>1493640</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>237600</xdr:rowOff>
     </xdr:to>
@@ -1015,7 +994,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14040" y="173880"/>
-          <a:ext cx="1479960" cy="642600"/>
+          <a:ext cx="1479600" cy="642600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1041,9 +1020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1057,7 +1036,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="840960" y="1533240"/>
-          <a:ext cx="13309560" cy="3457080"/>
+          <a:ext cx="13309200" cy="3456720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1078,9 +1057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1094,7 +1073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="821880" y="7210080"/>
-          <a:ext cx="13309560" cy="3333600"/>
+          <a:ext cx="13309200" cy="3333240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1114,10 +1093,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1048576" activeCellId="0" sqref="B1048576"/>
+      <selection pane="topLeft" activeCell="AMJ22" activeCellId="0" sqref="AMJ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1134,7 +1113,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="1.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10"/>
@@ -1157,7 +1136,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="6"/>
       <c r="H1" s="9" t="str">
-        <f aca="false">IF(AND(O3&gt;0,O4&gt;0,R21&gt;0,S21&gt;0),TEXT(O3,"YYYYMMDD")&amp;"-"&amp;TEXT(O4,"000")&amp;LEFT(R3,1)&amp;LEFT(R4,1)&amp;"-"&amp;E4,"Please complete")</f>
+        <f aca="false">IF(AND(O3&gt;0,O4&gt;0,R22&gt;0,S22&gt;0),TEXT(O3,"YYYYMMDD")&amp;"-"&amp;TEXT(O4,"000")&amp;LEFT(R3,1)&amp;LEFT(R4,1)&amp;"-"&amp;E4,"Please complete")</f>
         <v>Please complete</v>
       </c>
       <c r="J1" s="10"/>
@@ -1188,75 +1167,75 @@
       <c r="O2" s="22"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="23"/>
+      <c r="S2" s="20"/>
       <c r="T2" s="20"/>
-      <c r="U2" s="23"/>
+      <c r="U2" s="20"/>
       <c r="V2" s="18"/>
     </row>
     <row r="3" s="19" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="18"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="27" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="27"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
       <c r="Q3" s="15"/>
-      <c r="R3" s="31" t="s">
+      <c r="R3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="32"/>
-      <c r="U3" s="32"/>
+      <c r="S3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18"/>
     </row>
     <row r="4" s="19" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
       <c r="Q4" s="15"/>
-      <c r="R4" s="34" t="s">
+      <c r="R4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="32"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18"/>
     </row>
     <row r="5" s="19" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="18"/>
@@ -1268,683 +1247,719 @@
       <c r="V5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="39" t="s">
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="39"/>
-      <c r="J6" s="40" t="s">
+      <c r="I6" s="38"/>
+      <c r="J6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="39" t="s">
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="40" t="s">
+      <c r="N6" s="38"/>
+      <c r="O6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="43" t="s">
+      <c r="P6" s="39"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="44" t="s">
+      <c r="S6" s="42"/>
+      <c r="T6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="44"/>
+      <c r="U6" s="43"/>
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="47" t="s">
+      <c r="G7" s="40"/>
+      <c r="H7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="48" t="s">
+      <c r="K7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="47" t="s">
+      <c r="L7" s="40"/>
+      <c r="M7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="48" t="s">
+      <c r="O7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="48" t="s">
+      <c r="P7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="49" t="s">
+      <c r="Q7" s="40"/>
+      <c r="R7" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S7" s="49" t="s">
+      <c r="S7" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="50" t="s">
+      <c r="T7" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="50" t="s">
+      <c r="U7" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53" t="n">
+      <c r="B8" s="45"/>
+      <c r="C8" s="51" t="n">
         <v>10</v>
       </c>
-      <c r="D8" s="54" t="n">
+      <c r="D8" s="52" t="n">
         <v>0.25</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="53" t="n">
+      <c r="F8" s="54"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="51" t="n">
         <v>50</v>
       </c>
-      <c r="I8" s="54" t="n">
+      <c r="I8" s="52" t="n">
         <v>12.5</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="53" t="n">
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="51" t="n">
         <v>100</v>
       </c>
-      <c r="N8" s="54" t="n">
+      <c r="N8" s="52" t="n">
         <v>50</v>
       </c>
-      <c r="O8" s="55" t="s">
+      <c r="O8" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="59" t="s">
+      <c r="P8" s="54"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61" t="s">
+      <c r="S8" s="58"/>
+      <c r="T8" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="U8" s="62"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="63" t="s">
+      <c r="U8" s="60"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="59" t="n">
+      <c r="B9" s="45"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="57" t="n">
         <f aca="false">+C9+H9+M9</f>
         <v>0</v>
       </c>
-      <c r="S9" s="60" t="n">
+      <c r="S9" s="58" t="n">
         <f aca="false">+D9+I9+N9</f>
         <v>0</v>
       </c>
-      <c r="T9" s="61" t="n">
+      <c r="T9" s="59" t="n">
         <f aca="false">+E9+J9+O9</f>
         <v>0</v>
       </c>
-      <c r="U9" s="62" t="n">
+      <c r="U9" s="60" t="n">
         <f aca="false">+F9+K9+P9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="59" t="n">
+      <c r="B10" s="45"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="57" t="n">
         <f aca="false">+C10+H10+M10</f>
         <v>0</v>
       </c>
-      <c r="S10" s="60" t="n">
+      <c r="S10" s="58" t="n">
         <f aca="false">+D10+I10+N10</f>
         <v>0</v>
       </c>
-      <c r="T10" s="61" t="n">
+      <c r="T10" s="59" t="n">
         <f aca="false">+E10+J10+O10</f>
         <v>0</v>
       </c>
-      <c r="U10" s="62" t="n">
+      <c r="U10" s="60" t="n">
         <f aca="false">+F10+K10+P10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="63" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="59" t="n">
+      <c r="B11" s="45"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="57" t="n">
         <f aca="false">+C11+H11+M11</f>
         <v>0</v>
       </c>
-      <c r="S11" s="60" t="n">
+      <c r="S11" s="58" t="n">
         <f aca="false">+D11+I11+N11</f>
         <v>0</v>
       </c>
-      <c r="T11" s="61" t="n">
+      <c r="T11" s="59" t="n">
         <f aca="false">+E11+J11+O11</f>
         <v>0</v>
       </c>
-      <c r="U11" s="62" t="n">
+      <c r="U11" s="60" t="n">
         <f aca="false">+F11+K11+P11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59" t="n">
+      <c r="B12" s="45"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="57" t="n">
         <f aca="false">+C12+H12+M12</f>
         <v>0</v>
       </c>
-      <c r="S12" s="60" t="n">
+      <c r="S12" s="58" t="n">
         <f aca="false">+D12+I12+N12</f>
         <v>0</v>
       </c>
-      <c r="T12" s="61" t="n">
+      <c r="T12" s="59" t="n">
         <f aca="false">+E12+J12+O12</f>
         <v>0</v>
       </c>
-      <c r="U12" s="62" t="n">
+      <c r="U12" s="60" t="n">
         <f aca="false">+F12+K12+P12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="63" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="59" t="n">
+      <c r="B13" s="45"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="57" t="n">
         <f aca="false">+C13+H13+M13</f>
         <v>0</v>
       </c>
-      <c r="S13" s="60" t="n">
+      <c r="S13" s="58" t="n">
         <f aca="false">+D13+I13+N13</f>
         <v>0</v>
       </c>
-      <c r="T13" s="61" t="n">
+      <c r="T13" s="59" t="n">
         <f aca="false">+E13+J13+O13</f>
         <v>0</v>
       </c>
-      <c r="U13" s="62" t="n">
+      <c r="U13" s="60" t="n">
         <f aca="false">+F13+K13+P13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="63" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="59" t="n">
+      <c r="B14" s="45"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="57" t="n">
         <f aca="false">+C14+H14+M14</f>
         <v>0</v>
       </c>
-      <c r="S14" s="60" t="n">
+      <c r="S14" s="58" t="n">
         <f aca="false">+D14+I14+N14</f>
         <v>0</v>
       </c>
-      <c r="T14" s="61" t="n">
+      <c r="T14" s="59" t="n">
         <f aca="false">+E14+J14+O14</f>
         <v>0</v>
       </c>
-      <c r="U14" s="62" t="n">
+      <c r="U14" s="60" t="n">
         <f aca="false">+F14+K14+P14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="63" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="59" t="n">
+      <c r="B15" s="45"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="57" t="n">
         <f aca="false">+C15+H15+M15</f>
         <v>0</v>
       </c>
-      <c r="S15" s="60" t="n">
+      <c r="S15" s="58" t="n">
         <f aca="false">+D15+I15+N15</f>
         <v>0</v>
       </c>
-      <c r="T15" s="61" t="n">
+      <c r="T15" s="59" t="n">
         <f aca="false">+E15+J15+O15</f>
         <v>0</v>
       </c>
-      <c r="U15" s="62" t="n">
+      <c r="U15" s="60" t="n">
         <f aca="false">+F15+K15+P15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="63" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="59" t="n">
+      <c r="B16" s="45"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="57" t="n">
         <f aca="false">+C16+H16+M16</f>
         <v>0</v>
       </c>
-      <c r="S16" s="60" t="n">
+      <c r="S16" s="58" t="n">
         <f aca="false">+D16+I16+N16</f>
         <v>0</v>
       </c>
-      <c r="T16" s="61" t="n">
+      <c r="T16" s="59" t="n">
         <f aca="false">+E16+J16+O16</f>
         <v>0</v>
       </c>
-      <c r="U16" s="62" t="n">
+      <c r="U16" s="60" t="n">
         <f aca="false">+F16+K16+P16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="63" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="59" t="n">
+      <c r="B17" s="45"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="57" t="n">
         <f aca="false">+C17+H17+M17</f>
         <v>0</v>
       </c>
-      <c r="S17" s="60" t="n">
+      <c r="S17" s="58" t="n">
         <f aca="false">+D17+I17+N17</f>
         <v>0</v>
       </c>
-      <c r="T17" s="61" t="n">
+      <c r="T17" s="59" t="n">
         <f aca="false">+E17+J17+O17</f>
         <v>0</v>
       </c>
-      <c r="U17" s="62" t="n">
+      <c r="U17" s="60" t="n">
         <f aca="false">+F17+K17+P17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="63" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="59" t="n">
+      <c r="B18" s="45"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="57" t="n">
         <f aca="false">+C18+H18+M18</f>
         <v>0</v>
       </c>
-      <c r="S18" s="60" t="n">
+      <c r="S18" s="58" t="n">
         <f aca="false">+D18+I18+N18</f>
         <v>0</v>
       </c>
-      <c r="T18" s="61" t="n">
+      <c r="T18" s="59" t="n">
         <f aca="false">+E18+J18+O18</f>
         <v>0</v>
       </c>
-      <c r="U18" s="62" t="n">
+      <c r="U18" s="60" t="n">
         <f aca="false">+F18+K18+P18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="63" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="59" t="n">
+      <c r="B19" s="45"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="57" t="n">
         <f aca="false">+C19+H19+M19</f>
         <v>0</v>
       </c>
-      <c r="S19" s="60" t="n">
+      <c r="S19" s="58" t="n">
         <f aca="false">+D19+I19+N19</f>
         <v>0</v>
       </c>
-      <c r="T19" s="61" t="n">
+      <c r="T19" s="59" t="n">
         <f aca="false">+E19+J19+O19</f>
         <v>0</v>
       </c>
-      <c r="U19" s="62" t="n">
+      <c r="U19" s="60" t="n">
         <f aca="false">+F19+K19+P19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="63" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="59" t="n">
+      <c r="B20" s="45"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="57" t="n">
         <f aca="false">+C20+H20+M20</f>
         <v>0</v>
       </c>
-      <c r="S20" s="60" t="n">
+      <c r="S20" s="58" t="n">
         <f aca="false">+D20+I20+N20</f>
         <v>0</v>
       </c>
-      <c r="T20" s="61" t="n">
+      <c r="T20" s="59" t="n">
         <f aca="false">+E20+J20+O20</f>
         <v>0</v>
       </c>
-      <c r="U20" s="62" t="n">
+      <c r="U20" s="60" t="n">
         <f aca="false">+F20+K20+P20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="64" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="65" t="n">
-        <f aca="false">SUM(C9:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="66" t="n">
-        <f aca="false">SUM(D9:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="65" t="n">
-        <f aca="false">SUM(E9:E20)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="66" t="n">
-        <f aca="false">SUM(F9:F20)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="67"/>
-      <c r="H21" s="65" t="n">
-        <f aca="false">SUM(H9:H20)</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="66" t="n">
-        <f aca="false">SUM(I9:I20)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="65" t="n">
-        <f aca="false">SUM(J9:J20)</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="66" t="n">
-        <f aca="false">SUM(K9:K20)</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="67"/>
-      <c r="M21" s="65" t="n">
-        <f aca="false">SUM(M9:M20)</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="66" t="n">
-        <f aca="false">SUM(N9:N20)</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="65" t="n">
-        <f aca="false">SUM(O9:O20)</f>
-        <v>0</v>
-      </c>
-      <c r="P21" s="66" t="n">
-        <f aca="false">SUM(P9:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="67"/>
-      <c r="R21" s="65" t="n">
-        <f aca="false">SUM(R9:R20)</f>
-        <v>0</v>
-      </c>
-      <c r="S21" s="66" t="n">
-        <f aca="false">SUM(S9:S20)</f>
-        <v>0</v>
-      </c>
-      <c r="T21" s="65" t="n">
-        <f aca="false">SUM(T9:T20)</f>
-        <v>0</v>
-      </c>
-      <c r="U21" s="66" t="n">
-        <f aca="false">SUM(U9:U20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" s="19" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="68" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="57" t="n">
+        <f aca="false">+C21+H21+M21</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="58" t="n">
+        <f aca="false">+D21+I21+N21</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="59" t="n">
+        <f aca="false">+E21+J21+O21</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="60" t="n">
+        <f aca="false">+F21+K21+P21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="L22" s="15"/>
-      <c r="N22" s="69"/>
-      <c r="O22" s="69"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="69"/>
-      <c r="S22" s="69"/>
-      <c r="T22" s="71"/>
-      <c r="U22" s="71"/>
-      <c r="V22" s="18"/>
+      <c r="C22" s="63" t="n">
+        <f aca="false">SUM(C9:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="64" t="n">
+        <f aca="false">SUM(D9:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="63" t="n">
+        <f aca="false">SUM(E9:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="64" t="n">
+        <f aca="false">SUM(F9:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="65"/>
+      <c r="H22" s="63" t="n">
+        <f aca="false">SUM(H9:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="64" t="n">
+        <f aca="false">SUM(I9:I21)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="63" t="n">
+        <f aca="false">SUM(J9:J21)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="64" t="n">
+        <f aca="false">SUM(K9:K21)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="65"/>
+      <c r="M22" s="63" t="n">
+        <f aca="false">SUM(M9:M21)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="64" t="n">
+        <f aca="false">SUM(N9:N21)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="63" t="n">
+        <f aca="false">SUM(O9:O21)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="64" t="n">
+        <f aca="false">SUM(P9:P21)</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="65"/>
+      <c r="R22" s="63" t="n">
+        <f aca="false">SUM(R9:R21)</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="64" t="n">
+        <f aca="false">SUM(S9:S21)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="63" t="n">
+        <f aca="false">SUM(T9:T21)</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="64" t="n">
+        <f aca="false">SUM(U9:U21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" s="19" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="L23" s="15"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="68"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+      <c r="T23" s="69"/>
+      <c r="U23" s="69"/>
+      <c r="V23" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="20">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -1967,28 +1982,33 @@
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="T6:U6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G16:G20 L16:L20 S17:S20 U17:U20">
+  <conditionalFormatting sqref="G8 L8 S8 U8 G21 L21">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G10 G12 G14 L8:L10 L12 L14 S8 U8">
+  <conditionalFormatting sqref="G16:G20 L16:L20 S17:S20 U17:U20">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11 G13 G15 L11 L13 L15">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+  <conditionalFormatting sqref="G9:G10 G12 G14 L9:L10 L12 L14 G21 L21">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11 G13 G15 L11 L13 L15 S21 U21">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11:S16 U11:U16">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9:S10 U9:U10">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+  <conditionalFormatting sqref="S9:S10 U9:U10 S21 U21">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2031,23 +2051,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="72" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="72" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="70" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="70" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="73" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
-        <v>36</v>
+    <row r="1" s="71" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="71" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="72" t="s">
-        <v>37</v>
+      <c r="A2" s="70" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="72" t="s">
-        <v>38</v>
+      <c r="A3" s="70" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2074,63 +2094,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="74" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="72" width="9.14"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="B2" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="74" t="s">
-        <v>40</v>
+      <c r="B4" s="72" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="74" t="s">
-        <v>41</v>
+      <c r="B26" s="72" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="74" t="s">
-        <v>42</v>
+      <c r="B28" s="72" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="74" t="s">
-        <v>43</v>
+      <c r="B30" s="72" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="74" t="s">
-        <v>44</v>
+      <c r="B31" s="72" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="74" t="s">
-        <v>45</v>
+      <c r="B32" s="72" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="74" t="s">
-        <v>46</v>
+      <c r="B55" s="72" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="74" t="s">
-        <v>47</v>
+      <c r="B57" s="72" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Italy to the Secured Mail Maifest.
</commit_message>
<xml_diff>
--- a/spring_manifest/views/file_manifest/secure_mail_manifest_template.xlsx
+++ b/spring_manifest/views/file_manifest/secure_mail_manifest_template.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Instructions" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Priority Mail'!$A$1:$X$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Priority Mail'!$A$1:$X$24</definedName>
     <definedName function="false" hidden="false" name="CountryList" vbProcedure="false">data!#ref!</definedName>
     <definedName function="false" hidden="false" name="Format" vbProcedure="false">data!#ref!</definedName>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t xml:space="preserve">International Manifest</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
   </si>
   <si>
     <t xml:space="preserve">Rest of EU</t>
@@ -978,7 +981,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1493640</xdr:colOff>
+      <xdr:colOff>1493280</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>237600</xdr:rowOff>
     </xdr:to>
@@ -994,7 +997,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14040" y="173880"/>
-          <a:ext cx="1479600" cy="642600"/>
+          <a:ext cx="1479240" cy="642600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1020,9 +1023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1036,7 +1039,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="840960" y="1533240"/>
-          <a:ext cx="13309200" cy="3456720"/>
+          <a:ext cx="13308840" cy="3456360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1057,9 +1060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>313560</xdr:colOff>
+      <xdr:colOff>313200</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1073,7 +1076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="821880" y="7210080"/>
-          <a:ext cx="13309200" cy="3333240"/>
+          <a:ext cx="13308840" cy="3332880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,10 +1096,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMJ22" activeCellId="0" sqref="AMJ22"/>
+      <selection pane="topLeft" activeCell="F1048576" activeCellId="0" sqref="F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1136,7 +1139,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="6"/>
       <c r="H1" s="9" t="str">
-        <f aca="false">IF(AND(O3&gt;0,O4&gt;0,R22&gt;0,S22&gt;0),TEXT(O3,"YYYYMMDD")&amp;"-"&amp;TEXT(O4,"000")&amp;LEFT(R3,1)&amp;LEFT(R4,1)&amp;"-"&amp;E4,"Please complete")</f>
+        <f aca="false">IF(AND(O3&gt;0,O4&gt;0,R23&gt;0,S23&gt;0),TEXT(O3,"YYYYMMDD")&amp;"-"&amp;TEXT(O4,"000")&amp;LEFT(R3,1)&amp;LEFT(R4,1)&amp;"-"&amp;E4,"Please complete")</f>
         <v>Please complete</v>
       </c>
       <c r="J1" s="10"/>
@@ -1871,93 +1874,125 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="63" t="n">
-        <f aca="false">SUM(C9:C21)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="64" t="n">
-        <f aca="false">SUM(D9:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="63" t="n">
-        <f aca="false">SUM(E9:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="64" t="n">
-        <f aca="false">SUM(F9:F21)</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="63" t="n">
-        <f aca="false">SUM(H9:H21)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="64" t="n">
-        <f aca="false">SUM(I9:I21)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="63" t="n">
-        <f aca="false">SUM(J9:J21)</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="64" t="n">
-        <f aca="false">SUM(K9:K21)</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="65"/>
-      <c r="M22" s="63" t="n">
-        <f aca="false">SUM(M9:M21)</f>
-        <v>0</v>
-      </c>
-      <c r="N22" s="64" t="n">
-        <f aca="false">SUM(N9:N21)</f>
-        <v>0</v>
-      </c>
-      <c r="O22" s="63" t="n">
-        <f aca="false">SUM(O9:O21)</f>
-        <v>0</v>
-      </c>
-      <c r="P22" s="64" t="n">
-        <f aca="false">SUM(P9:P21)</f>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="63" t="n">
-        <f aca="false">SUM(R9:R21)</f>
-        <v>0</v>
-      </c>
-      <c r="S22" s="64" t="n">
-        <f aca="false">SUM(S9:S21)</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="63" t="n">
-        <f aca="false">SUM(T9:T21)</f>
-        <v>0</v>
-      </c>
-      <c r="U22" s="64" t="n">
-        <f aca="false">SUM(U9:U21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" s="19" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="66" t="s">
+      <c r="B22" s="45"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="58"/>
+      <c r="T22" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" s="60" t="n">
+        <f aca="false">+F22+K22+P22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="L23" s="15"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="68"/>
-      <c r="R23" s="67"/>
-      <c r="S23" s="67"/>
-      <c r="T23" s="69"/>
-      <c r="U23" s="69"/>
-      <c r="V23" s="18"/>
+      <c r="C23" s="63" t="n">
+        <f aca="false">SUM(C9:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="64" t="n">
+        <f aca="false">SUM(D9:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="63" t="n">
+        <f aca="false">SUM(E9:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="64" t="n">
+        <f aca="false">SUM(F9:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="65"/>
+      <c r="H23" s="63" t="n">
+        <f aca="false">SUM(H9:H22)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="64" t="n">
+        <f aca="false">SUM(I9:I22)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="63" t="n">
+        <f aca="false">SUM(J9:J22)</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="64" t="n">
+        <f aca="false">SUM(K9:K22)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="65"/>
+      <c r="M23" s="63" t="n">
+        <f aca="false">SUM(M9:M22)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="64" t="n">
+        <f aca="false">SUM(N9:N22)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="63" t="n">
+        <f aca="false">SUM(O9:O22)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="64" t="n">
+        <f aca="false">SUM(P9:P22)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="63" t="n">
+        <f aca="false">SUM(R9:R22)</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="64" t="n">
+        <f aca="false">SUM(S9:S22)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="63" t="n">
+        <f aca="false">SUM(T9:T22)</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="64" t="n">
+        <f aca="false">SUM(U9:U22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" s="19" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="L24" s="15"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -1982,7 +2017,7 @@
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="T6:U6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G8 L8 S8 U8 G21 L21">
+  <conditionalFormatting sqref="G8 L8 S8 U8 G21:G22 L21:L22">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -1992,12 +2027,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G10 G12 G14 L9:L10 L12 L14 G21 L21">
+  <conditionalFormatting sqref="G9:G10 G12 G14 L9:L10 L12 L14 G21:G22 L21:L22">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11 G13 G15 L11 L13 L15 S21 U21">
+  <conditionalFormatting sqref="G11 G13 G15 L11 L13 L15 S21:S22 U21:U22">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
@@ -2007,7 +2042,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9:S10 U9:U10 S21 U21">
+  <conditionalFormatting sqref="S9:S10 U9:U10 S21:S22 U21:U22">
     <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
     </cfRule>
@@ -2057,17 +2092,17 @@
   <sheetData>
     <row r="1" s="71" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="70" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="70" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2134,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="73" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="73"/>
       <c r="D2" s="73"/>
@@ -2115,42 +2150,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="72" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="72" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="72" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="72" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="72" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="72" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="72" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="72" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>